<commit_message>
refactor: adjust to new payer tracking logic
</commit_message>
<xml_diff>
--- a/public/lockup_import_example.xlsx
+++ b/public/lockup_import_example.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="127">
   <si>
     <t>Beneficiary account id
 on the NEAR protocol</t>
@@ -35,15 +35,9 @@
 If emtpy, then it will be impossible 
 to terminate the lockup.
 Must be ahead of the termination schedule
-at each moment in time</t>
-  </si>
-  <si>
-    <t>Account that can invoke 
-lockup termination.
-Unvested tokens will return 
-to terminator on terminate.
-Must be present if and only if
-the vesting schedule is present.</t>
+at each moment in time
+After termination unvested amount 
+will return to the payer.</t>
   </si>
   <si>
     <t>account_id</t>
@@ -58,9 +52,6 @@
     <t>vesting_schedule</t>
   </si>
   <si>
-    <t>terminator_id</t>
-  </si>
-  <si>
     <t>alice.near</t>
   </si>
   <si>
@@ -70,9 +61,6 @@
     <t>2022-05-01T08:00:00Z|P4Y|P1Y:25|P1Y</t>
   </si>
   <si>
-    <t>owner.near</t>
-  </si>
-  <si>
     <t>bob.near</t>
   </si>
   <si>
@@ -80,6 +68,9 @@
   </si>
   <si>
     <t>Copy and paste green region (INCLUDING HEADER ROW) to the form as test input</t>
+  </si>
+  <si>
+    <t>1999-12-31T23:59:59Z|PT0S|PT0S:25|PT1S</t>
   </si>
   <si>
     <t>Schedule ::= StartDate|TotalDuration|Cliff|ReleaseStepInterval
@@ -106,7 +97,13 @@
 See the checkpoints below</t>
   </si>
   <si>
+    <t>terminator_id</t>
+  </si>
+  <si>
     <t>2009-12-31T23:59:59Z|P4Y|P2Y:50|P1M</t>
+  </si>
+  <si>
+    <t>owner.near</t>
   </si>
   <si>
     <t>1999-12-31T23:59:59Z|P4Y|P2Y:50|P1M</t>
@@ -437,8 +434,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd hh:mm:ss"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000000000000000"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd hh:mm:ss"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -469,61 +467,61 @@
     <border/>
     <border>
       <left style="thick">
-        <color rgb="FF6AA84F"/>
+        <color rgb="FF34A853"/>
       </left>
       <top style="thick">
-        <color rgb="FF6AA84F"/>
+        <color rgb="FF34A853"/>
       </top>
     </border>
     <border>
       <top style="thick">
-        <color rgb="FF6AA84F"/>
+        <color rgb="FF34A853"/>
       </top>
     </border>
     <border>
       <right style="thick">
-        <color rgb="FF6AA84F"/>
+        <color rgb="FF34A853"/>
       </right>
       <top style="thick">
-        <color rgb="FF6AA84F"/>
+        <color rgb="FF34A853"/>
       </top>
     </border>
     <border>
       <left style="thick">
-        <color rgb="FF6AA84F"/>
+        <color rgb="FF34A853"/>
       </left>
     </border>
     <border>
       <right style="thick">
-        <color rgb="FF6AA84F"/>
+        <color rgb="FF34A853"/>
       </right>
     </border>
     <border>
       <left style="thick">
-        <color rgb="FF6AA84F"/>
+        <color rgb="FF34A853"/>
       </left>
       <bottom style="thick">
-        <color rgb="FF6AA84F"/>
+        <color rgb="FF34A853"/>
       </bottom>
     </border>
     <border>
       <bottom style="thick">
-        <color rgb="FF6AA84F"/>
+        <color rgb="FF34A853"/>
       </bottom>
     </border>
     <border>
       <right style="thick">
-        <color rgb="FF6AA84F"/>
+        <color rgb="FF34A853"/>
       </right>
       <bottom style="thick">
-        <color rgb="FF6AA84F"/>
+        <color rgb="FF34A853"/>
       </bottom>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -545,8 +543,8 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -557,8 +555,13 @@
     <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -805,69 +808,92 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="E2" s="1"/>
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1">
         <v>10000.25</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>13</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1"/>
     </row>
     <row r="4">
       <c r="A4" s="8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B4" s="9">
         <v>20000.49</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="D4" s="11"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="12">
+        <v>9000.000456789</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>17</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="E8" s="1"/>
     </row>
     <row r="12">
-      <c r="A12" s="12">
+      <c r="A12" s="13">
         <v>44682.333333333336</v>
       </c>
       <c r="B12" s="1">
@@ -875,7 +901,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="12">
+      <c r="A13" s="13">
         <v>45047.33332175926</v>
       </c>
       <c r="B13" s="1">
@@ -883,7 +909,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="12">
+      <c r="A14" s="13">
         <v>45047.333333333336</v>
       </c>
       <c r="B14" s="1">
@@ -891,7 +917,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="12">
+      <c r="A15" s="13">
         <v>45231.33332175926</v>
       </c>
       <c r="B15" s="1">
@@ -899,7 +925,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="12">
+      <c r="A16" s="13">
         <v>45231.333333333336</v>
       </c>
       <c r="B16" s="1">
@@ -907,7 +933,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="12">
+      <c r="A17" s="13">
         <v>45413.33332175926</v>
       </c>
       <c r="B17" s="1">
@@ -915,7 +941,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="12">
+      <c r="A18" s="13">
         <v>45413.333333333336</v>
       </c>
       <c r="B18" s="1">
@@ -923,7 +949,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="12">
+      <c r="A19" s="13">
         <v>45597.33332175926</v>
       </c>
       <c r="B19" s="1">
@@ -931,7 +957,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="12">
+      <c r="A20" s="13">
         <v>45597.333333333336</v>
       </c>
       <c r="B20" s="1">
@@ -939,7 +965,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="12">
+      <c r="A21" s="13">
         <v>45778.33332175926</v>
       </c>
       <c r="B21" s="1">
@@ -947,7 +973,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="12">
+      <c r="A22" s="13">
         <v>45778.333333333336</v>
       </c>
       <c r="B22" s="1">
@@ -955,7 +981,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="12">
+      <c r="A23" s="13">
         <v>45962.33332175926</v>
       </c>
       <c r="B23" s="1">
@@ -963,7 +989,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="12">
+      <c r="A24" s="13">
         <v>45962.333333333336</v>
       </c>
       <c r="B24" s="1">
@@ -971,7 +997,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="12">
+      <c r="A25" s="13">
         <v>46143.33332175926</v>
       </c>
       <c r="B25" s="1">
@@ -979,7 +1005,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="12">
+      <c r="A26" s="13">
         <v>46143.333333333336</v>
       </c>
       <c r="B26" s="1">
@@ -988,7 +1014,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="A8:D8"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1013,53 +1039,53 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1">
         <v>30000.0</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>18</v>
+      <c r="C2" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1">
         <v>100000.0</v>
       </c>
-      <c r="C3" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="13"/>
+      <c r="C3" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="14"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1">
         <v>100000.0</v>
@@ -1071,12 +1097,12 @@
         <v>21</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1">
         <v>30000.0</v>
@@ -1088,24 +1114,24 @@
         <v>21</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="E8" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9">
@@ -1144,1753 +1170,1753 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="E13" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="15" t="s">
         <v>25</v>
       </c>
       <c r="B14" s="1">
         <v>10000.0</v>
       </c>
-      <c r="C14" s="13" t="s">
-        <v>18</v>
+      <c r="C14" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="15" t="s">
         <v>26</v>
       </c>
       <c r="B15" s="1">
         <v>20000.0</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="15" t="s">
         <v>27</v>
       </c>
       <c r="B16" s="1">
         <v>30000.0</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="15" t="s">
         <v>28</v>
       </c>
       <c r="B17" s="1">
         <v>40000.0</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="15" t="s">
         <v>29</v>
       </c>
       <c r="B18" s="1">
         <v>50000.0</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
         <v>30</v>
       </c>
       <c r="B19" s="1">
         <v>60000.0</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="15" t="s">
         <v>31</v>
       </c>
       <c r="B20" s="1">
         <v>70000.0</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="15" t="s">
         <v>32</v>
       </c>
       <c r="B21" s="1">
         <v>80000.0</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B22" s="1">
         <v>90000.0</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="15" t="s">
         <v>34</v>
       </c>
       <c r="B23" s="1">
         <v>100000.0</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="15" t="s">
         <v>35</v>
       </c>
       <c r="B24" s="1">
         <v>110000.0</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="15" t="s">
         <v>36</v>
       </c>
       <c r="B25" s="1">
         <v>120000.0</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="15" t="s">
         <v>37</v>
       </c>
       <c r="B26" s="1">
         <v>130000.0</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="15" t="s">
         <v>38</v>
       </c>
       <c r="B27" s="1">
         <v>140000.0</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="15" t="s">
         <v>39</v>
       </c>
       <c r="B28" s="1">
         <v>150000.0</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="15" t="s">
         <v>40</v>
       </c>
       <c r="B29" s="1">
         <v>160000.0</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="15" t="s">
         <v>41</v>
       </c>
       <c r="B30" s="1">
         <v>170000.0</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="14" t="s">
+      <c r="A31" s="15" t="s">
         <v>42</v>
       </c>
       <c r="B31" s="1">
         <v>180000.0</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="15" t="s">
         <v>43</v>
       </c>
       <c r="B32" s="1">
         <v>190000.0</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="14" t="s">
+      <c r="A33" s="15" t="s">
         <v>44</v>
       </c>
       <c r="B33" s="1">
         <v>200000.0</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="14" t="s">
+      <c r="A34" s="15" t="s">
         <v>45</v>
       </c>
       <c r="B34" s="1">
         <v>210000.0</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C34" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D34" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="14" t="s">
+      <c r="A35" s="15" t="s">
         <v>46</v>
       </c>
       <c r="B35" s="1">
         <v>220000.0</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D35" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="14" t="s">
+      <c r="A36" s="15" t="s">
         <v>47</v>
       </c>
       <c r="B36" s="1">
         <v>230000.0</v>
       </c>
-      <c r="C36" s="13" t="s">
+      <c r="C36" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D36" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="15" t="s">
         <v>48</v>
       </c>
       <c r="B37" s="1">
         <v>240000.0</v>
       </c>
-      <c r="C37" s="13" t="s">
+      <c r="C37" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D37" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="14" t="s">
+      <c r="A38" s="15" t="s">
         <v>49</v>
       </c>
       <c r="B38" s="1">
         <v>250000.0</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="C38" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="14" t="s">
+      <c r="A39" s="15" t="s">
         <v>50</v>
       </c>
       <c r="B39" s="1">
         <v>260000.0</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C39" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="14" t="s">
+      <c r="A40" s="15" t="s">
         <v>51</v>
       </c>
       <c r="B40" s="1">
         <v>270000.0</v>
       </c>
-      <c r="C40" s="13" t="s">
+      <c r="C40" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="14" t="s">
+      <c r="A41" s="15" t="s">
         <v>52</v>
       </c>
       <c r="B41" s="1">
         <v>280000.0</v>
       </c>
-      <c r="C41" s="13" t="s">
+      <c r="C41" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="14" t="s">
+      <c r="A42" s="15" t="s">
         <v>53</v>
       </c>
       <c r="B42" s="1">
         <v>290000.0</v>
       </c>
-      <c r="C42" s="13" t="s">
+      <c r="C42" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D42" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="14" t="s">
+      <c r="A43" s="15" t="s">
         <v>54</v>
       </c>
       <c r="B43" s="1">
         <v>300000.0</v>
       </c>
-      <c r="C43" s="13" t="s">
+      <c r="C43" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="14" t="s">
+      <c r="A44" s="15" t="s">
         <v>55</v>
       </c>
       <c r="B44" s="1">
         <v>310000.0</v>
       </c>
-      <c r="C44" s="13" t="s">
+      <c r="C44" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D44" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="14" t="s">
+      <c r="A45" s="15" t="s">
         <v>56</v>
       </c>
       <c r="B45" s="1">
         <v>320000.0</v>
       </c>
-      <c r="C45" s="13" t="s">
+      <c r="C45" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D45" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="14" t="s">
+      <c r="A46" s="15" t="s">
         <v>57</v>
       </c>
       <c r="B46" s="1">
         <v>330000.0</v>
       </c>
-      <c r="C46" s="13" t="s">
+      <c r="C46" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D46" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="14" t="s">
+      <c r="A47" s="15" t="s">
         <v>58</v>
       </c>
       <c r="B47" s="1">
         <v>340000.0</v>
       </c>
-      <c r="C47" s="13" t="s">
+      <c r="C47" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D47" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="14" t="s">
+      <c r="A48" s="15" t="s">
         <v>59</v>
       </c>
       <c r="B48" s="1">
         <v>350000.0</v>
       </c>
-      <c r="C48" s="13" t="s">
+      <c r="C48" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D48" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="14" t="s">
+      <c r="A49" s="15" t="s">
         <v>60</v>
       </c>
       <c r="B49" s="1">
         <v>360000.0</v>
       </c>
-      <c r="C49" s="13" t="s">
+      <c r="C49" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D49" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="14" t="s">
+      <c r="A50" s="15" t="s">
         <v>61</v>
       </c>
       <c r="B50" s="1">
         <v>370000.0</v>
       </c>
-      <c r="C50" s="13" t="s">
+      <c r="C50" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D50" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="14" t="s">
+      <c r="A51" s="15" t="s">
         <v>62</v>
       </c>
       <c r="B51" s="1">
         <v>380000.0</v>
       </c>
-      <c r="C51" s="13" t="s">
+      <c r="C51" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D51" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="14" t="s">
+      <c r="A52" s="15" t="s">
         <v>63</v>
       </c>
       <c r="B52" s="1">
         <v>390000.0</v>
       </c>
-      <c r="C52" s="13" t="s">
+      <c r="C52" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D52" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="14" t="s">
+      <c r="A53" s="15" t="s">
         <v>64</v>
       </c>
       <c r="B53" s="1">
         <v>400000.0</v>
       </c>
-      <c r="C53" s="13" t="s">
+      <c r="C53" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D53" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="14" t="s">
+      <c r="A54" s="15" t="s">
         <v>65</v>
       </c>
       <c r="B54" s="1">
         <v>410000.0</v>
       </c>
-      <c r="C54" s="13" t="s">
+      <c r="C54" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D54" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="14" t="s">
+      <c r="A55" s="15" t="s">
         <v>66</v>
       </c>
       <c r="B55" s="1">
         <v>420000.0</v>
       </c>
-      <c r="C55" s="13" t="s">
+      <c r="C55" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D55" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="14" t="s">
+      <c r="A56" s="15" t="s">
         <v>67</v>
       </c>
       <c r="B56" s="1">
         <v>430000.0</v>
       </c>
-      <c r="C56" s="13" t="s">
+      <c r="C56" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D56" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="14" t="s">
+      <c r="A57" s="15" t="s">
         <v>68</v>
       </c>
       <c r="B57" s="1">
         <v>440000.0</v>
       </c>
-      <c r="C57" s="13" t="s">
+      <c r="C57" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D57" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="14" t="s">
+      <c r="A58" s="15" t="s">
         <v>69</v>
       </c>
       <c r="B58" s="1">
         <v>450000.0</v>
       </c>
-      <c r="C58" s="13" t="s">
+      <c r="C58" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D58" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="14" t="s">
+      <c r="A59" s="15" t="s">
         <v>70</v>
       </c>
       <c r="B59" s="1">
         <v>460000.0</v>
       </c>
-      <c r="C59" s="13" t="s">
+      <c r="C59" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D59" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="14" t="s">
+      <c r="A60" s="15" t="s">
         <v>71</v>
       </c>
       <c r="B60" s="1">
         <v>470000.0</v>
       </c>
-      <c r="C60" s="13" t="s">
+      <c r="C60" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D60" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="14" t="s">
+      <c r="A61" s="15" t="s">
         <v>72</v>
       </c>
       <c r="B61" s="1">
         <v>480000.0</v>
       </c>
-      <c r="C61" s="13" t="s">
+      <c r="C61" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D61" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="14" t="s">
+      <c r="A62" s="15" t="s">
         <v>73</v>
       </c>
       <c r="B62" s="1">
         <v>490000.0</v>
       </c>
-      <c r="C62" s="13" t="s">
+      <c r="C62" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D62" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="14" t="s">
+      <c r="A63" s="15" t="s">
         <v>74</v>
       </c>
       <c r="B63" s="1">
         <v>500000.0</v>
       </c>
-      <c r="C63" s="13" t="s">
+      <c r="C63" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D63" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="14" t="s">
+      <c r="A64" s="15" t="s">
         <v>75</v>
       </c>
       <c r="B64" s="1">
         <v>510000.0</v>
       </c>
-      <c r="C64" s="13" t="s">
+      <c r="C64" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D64" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="14" t="s">
+      <c r="A65" s="15" t="s">
         <v>76</v>
       </c>
       <c r="B65" s="1">
         <v>520000.0</v>
       </c>
-      <c r="C65" s="13" t="s">
+      <c r="C65" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D65" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="14" t="s">
+      <c r="A66" s="15" t="s">
         <v>77</v>
       </c>
       <c r="B66" s="1">
         <v>530000.0</v>
       </c>
-      <c r="C66" s="13" t="s">
+      <c r="C66" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D66" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="14" t="s">
+      <c r="A67" s="15" t="s">
         <v>78</v>
       </c>
       <c r="B67" s="1">
         <v>540000.0</v>
       </c>
-      <c r="C67" s="13" t="s">
+      <c r="C67" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D67" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="14" t="s">
+      <c r="A68" s="15" t="s">
         <v>79</v>
       </c>
       <c r="B68" s="1">
         <v>550000.0</v>
       </c>
-      <c r="C68" s="13" t="s">
+      <c r="C68" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D68" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="14" t="s">
+      <c r="A69" s="15" t="s">
         <v>80</v>
       </c>
       <c r="B69" s="1">
         <v>560000.0</v>
       </c>
-      <c r="C69" s="13" t="s">
+      <c r="C69" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D69" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="14" t="s">
+      <c r="A70" s="15" t="s">
         <v>81</v>
       </c>
       <c r="B70" s="1">
         <v>570000.0</v>
       </c>
-      <c r="C70" s="13" t="s">
+      <c r="C70" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D70" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="14" t="s">
+      <c r="A71" s="15" t="s">
         <v>82</v>
       </c>
       <c r="B71" s="1">
         <v>580000.0</v>
       </c>
-      <c r="C71" s="13" t="s">
+      <c r="C71" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D71" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="14" t="s">
+      <c r="A72" s="15" t="s">
         <v>83</v>
       </c>
       <c r="B72" s="1">
         <v>590000.0</v>
       </c>
-      <c r="C72" s="13" t="s">
+      <c r="C72" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D72" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="14" t="s">
+      <c r="A73" s="15" t="s">
         <v>84</v>
       </c>
       <c r="B73" s="1">
         <v>600000.0</v>
       </c>
-      <c r="C73" s="13" t="s">
+      <c r="C73" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D73" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="14" t="s">
+      <c r="A74" s="15" t="s">
         <v>85</v>
       </c>
       <c r="B74" s="1">
         <v>610000.0</v>
       </c>
-      <c r="C74" s="13" t="s">
+      <c r="C74" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D74" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="14" t="s">
+      <c r="A75" s="15" t="s">
         <v>86</v>
       </c>
       <c r="B75" s="1">
         <v>620000.0</v>
       </c>
-      <c r="C75" s="13" t="s">
+      <c r="C75" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D75" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="14" t="s">
+      <c r="A76" s="15" t="s">
         <v>87</v>
       </c>
       <c r="B76" s="1">
         <v>630000.0</v>
       </c>
-      <c r="C76" s="13" t="s">
+      <c r="C76" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D76" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="14" t="s">
+      <c r="A77" s="15" t="s">
         <v>88</v>
       </c>
       <c r="B77" s="1">
         <v>640000.0</v>
       </c>
-      <c r="C77" s="13" t="s">
+      <c r="C77" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D77" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="14" t="s">
+      <c r="A78" s="15" t="s">
         <v>89</v>
       </c>
       <c r="B78" s="1">
         <v>650000.0</v>
       </c>
-      <c r="C78" s="13" t="s">
+      <c r="C78" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D78" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="14" t="s">
+      <c r="A79" s="15" t="s">
         <v>90</v>
       </c>
       <c r="B79" s="1">
         <v>660000.0</v>
       </c>
-      <c r="C79" s="13" t="s">
+      <c r="C79" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D79" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="14" t="s">
+      <c r="A80" s="15" t="s">
         <v>91</v>
       </c>
       <c r="B80" s="1">
         <v>670000.0</v>
       </c>
-      <c r="C80" s="13" t="s">
+      <c r="C80" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D80" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="14" t="s">
+      <c r="A81" s="15" t="s">
         <v>92</v>
       </c>
       <c r="B81" s="1">
         <v>680000.0</v>
       </c>
-      <c r="C81" s="13" t="s">
+      <c r="C81" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D81" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="14" t="s">
+      <c r="A82" s="15" t="s">
         <v>93</v>
       </c>
       <c r="B82" s="1">
         <v>690000.0</v>
       </c>
-      <c r="C82" s="13" t="s">
+      <c r="C82" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D82" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="14" t="s">
+      <c r="A83" s="15" t="s">
         <v>94</v>
       </c>
       <c r="B83" s="1">
         <v>700000.0</v>
       </c>
-      <c r="C83" s="13" t="s">
+      <c r="C83" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D83" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="14" t="s">
+      <c r="A84" s="15" t="s">
         <v>95</v>
       </c>
       <c r="B84" s="1">
         <v>710000.0</v>
       </c>
-      <c r="C84" s="13" t="s">
+      <c r="C84" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D84" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="14" t="s">
+      <c r="A85" s="15" t="s">
         <v>96</v>
       </c>
       <c r="B85" s="1">
         <v>720000.0</v>
       </c>
-      <c r="C85" s="13" t="s">
+      <c r="C85" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D85" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="14" t="s">
+      <c r="A86" s="15" t="s">
         <v>97</v>
       </c>
       <c r="B86" s="1">
         <v>730000.0</v>
       </c>
-      <c r="C86" s="13" t="s">
+      <c r="C86" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D86" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="14" t="s">
+      <c r="A87" s="15" t="s">
         <v>98</v>
       </c>
       <c r="B87" s="1">
         <v>740000.0</v>
       </c>
-      <c r="C87" s="13" t="s">
+      <c r="C87" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D87" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="14" t="s">
+      <c r="A88" s="15" t="s">
         <v>99</v>
       </c>
       <c r="B88" s="1">
         <v>750000.0</v>
       </c>
-      <c r="C88" s="13" t="s">
+      <c r="C88" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D88" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="14" t="s">
+      <c r="A89" s="15" t="s">
         <v>100</v>
       </c>
       <c r="B89" s="1">
         <v>760000.0</v>
       </c>
-      <c r="C89" s="13" t="s">
+      <c r="C89" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D89" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="14" t="s">
+      <c r="A90" s="15" t="s">
         <v>101</v>
       </c>
       <c r="B90" s="1">
         <v>770000.0</v>
       </c>
-      <c r="C90" s="13" t="s">
+      <c r="C90" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D90" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="14" t="s">
+      <c r="A91" s="15" t="s">
         <v>102</v>
       </c>
       <c r="B91" s="1">
         <v>780000.0</v>
       </c>
-      <c r="C91" s="13" t="s">
+      <c r="C91" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D91" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="14" t="s">
+      <c r="A92" s="15" t="s">
         <v>103</v>
       </c>
       <c r="B92" s="1">
         <v>790000.0</v>
       </c>
-      <c r="C92" s="13" t="s">
+      <c r="C92" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D92" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="14" t="s">
+      <c r="A93" s="15" t="s">
         <v>104</v>
       </c>
       <c r="B93" s="1">
         <v>800000.0</v>
       </c>
-      <c r="C93" s="13" t="s">
+      <c r="C93" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D93" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="14" t="s">
+      <c r="A94" s="15" t="s">
         <v>105</v>
       </c>
       <c r="B94" s="1">
         <v>810000.0</v>
       </c>
-      <c r="C94" s="13" t="s">
+      <c r="C94" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D94" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="14" t="s">
+      <c r="A95" s="15" t="s">
         <v>106</v>
       </c>
       <c r="B95" s="1">
         <v>820000.0</v>
       </c>
-      <c r="C95" s="13" t="s">
+      <c r="C95" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D95" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="14" t="s">
+      <c r="A96" s="15" t="s">
         <v>107</v>
       </c>
       <c r="B96" s="1">
         <v>830000.0</v>
       </c>
-      <c r="C96" s="13" t="s">
+      <c r="C96" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D96" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="14" t="s">
+      <c r="A97" s="15" t="s">
         <v>108</v>
       </c>
       <c r="B97" s="1">
         <v>840000.0</v>
       </c>
-      <c r="C97" s="13" t="s">
+      <c r="C97" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D97" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="14" t="s">
+      <c r="A98" s="15" t="s">
         <v>109</v>
       </c>
       <c r="B98" s="1">
         <v>850000.0</v>
       </c>
-      <c r="C98" s="13" t="s">
+      <c r="C98" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D98" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="14" t="s">
+      <c r="A99" s="15" t="s">
         <v>110</v>
       </c>
       <c r="B99" s="1">
         <v>860000.0</v>
       </c>
-      <c r="C99" s="13" t="s">
+      <c r="C99" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D99" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="14" t="s">
+      <c r="A100" s="15" t="s">
         <v>111</v>
       </c>
       <c r="B100" s="1">
         <v>870000.0</v>
       </c>
-      <c r="C100" s="13" t="s">
+      <c r="C100" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D100" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="14" t="s">
+      <c r="A101" s="15" t="s">
         <v>112</v>
       </c>
       <c r="B101" s="1">
         <v>880000.0</v>
       </c>
-      <c r="C101" s="13" t="s">
+      <c r="C101" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D101" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="14" t="s">
+      <c r="A102" s="15" t="s">
         <v>113</v>
       </c>
       <c r="B102" s="1">
         <v>890000.0</v>
       </c>
-      <c r="C102" s="13" t="s">
+      <c r="C102" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D102" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="14" t="s">
+      <c r="A103" s="15" t="s">
         <v>114</v>
       </c>
       <c r="B103" s="1">
         <v>900000.0</v>
       </c>
-      <c r="C103" s="13" t="s">
+      <c r="C103" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D103" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="104">
-      <c r="A104" s="14" t="s">
+      <c r="A104" s="15" t="s">
         <v>115</v>
       </c>
       <c r="B104" s="1">
         <v>910000.0</v>
       </c>
-      <c r="C104" s="13" t="s">
+      <c r="C104" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D104" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="14" t="s">
+      <c r="A105" s="15" t="s">
         <v>116</v>
       </c>
       <c r="B105" s="1">
         <v>920000.0</v>
       </c>
-      <c r="C105" s="13" t="s">
+      <c r="C105" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D105" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="14" t="s">
+      <c r="A106" s="15" t="s">
         <v>117</v>
       </c>
       <c r="B106" s="1">
         <v>930000.0</v>
       </c>
-      <c r="C106" s="13" t="s">
+      <c r="C106" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D106" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="14" t="s">
+      <c r="A107" s="15" t="s">
         <v>118</v>
       </c>
       <c r="B107" s="1">
         <v>940000.0</v>
       </c>
-      <c r="C107" s="13" t="s">
+      <c r="C107" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D107" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="108">
-      <c r="A108" s="14" t="s">
+      <c r="A108" s="15" t="s">
         <v>119</v>
       </c>
       <c r="B108" s="1">
         <v>950000.0</v>
       </c>
-      <c r="C108" s="13" t="s">
+      <c r="C108" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D108" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="14" t="s">
+      <c r="A109" s="15" t="s">
         <v>120</v>
       </c>
       <c r="B109" s="1">
         <v>960000.0</v>
       </c>
-      <c r="C109" s="13" t="s">
+      <c r="C109" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D109" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="110">
-      <c r="A110" s="14" t="s">
+      <c r="A110" s="15" t="s">
         <v>121</v>
       </c>
       <c r="B110" s="1">
         <v>970000.0</v>
       </c>
-      <c r="C110" s="13" t="s">
+      <c r="C110" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D110" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="111">
-      <c r="A111" s="14" t="s">
+      <c r="A111" s="15" t="s">
         <v>122</v>
       </c>
       <c r="B111" s="1">
         <v>980000.0</v>
       </c>
-      <c r="C111" s="13" t="s">
+      <c r="C111" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D111" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="14" t="s">
+      <c r="A112" s="15" t="s">
         <v>123</v>
       </c>
       <c r="B112" s="1">
         <v>990000.0</v>
       </c>
-      <c r="C112" s="13" t="s">
+      <c r="C112" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D112" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="113">
-      <c r="A113" s="14" t="s">
+      <c r="A113" s="15" t="s">
         <v>124</v>
       </c>
       <c r="B113" s="1">
         <v>1000000.0</v>
       </c>
-      <c r="C113" s="13" t="s">
+      <c r="C113" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D113" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="114">
-      <c r="A114" s="14" t="s">
+      <c r="A114" s="15" t="s">
         <v>125</v>
       </c>
       <c r="B114" s="1">
         <v>1010000.0</v>
       </c>
-      <c r="C114" s="13" t="s">
+      <c r="C114" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D114" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="115">
-      <c r="A115" s="14" t="s">
+      <c r="A115" s="15" t="s">
         <v>126</v>
       </c>
       <c r="B115" s="1">
         <v>1020000.0</v>
       </c>
-      <c r="C115" s="13" t="s">
+      <c r="C115" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D115" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>